<commit_message>
added in percentage and multiplier
</commit_message>
<xml_diff>
--- a/productImportExample.xlsx
+++ b/productImportExample.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sale\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian.gao\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8A161646-FB7A-43F3-9435-F5C8EC40A123}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16788" windowHeight="7632"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>name</t>
   </si>
@@ -133,12 +132,18 @@
   </si>
   <si>
     <t>5,10</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>multiplier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,26 +488,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="7" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" customWidth="1"/>
-    <col min="15" max="15" width="20.77734375" customWidth="1"/>
-    <col min="16" max="16" width="14.88671875" customWidth="1"/>
-    <col min="17" max="17" width="15" customWidth="1"/>
-    <col min="18" max="18" width="16.33203125" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
+    <col min="13" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
+    <col min="17" max="17" width="20.77734375" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" customWidth="1"/>
+    <col min="21" max="21" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -543,19 +548,25 @@
         <v>14</v>
       </c>
       <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>59</v>
       </c>
@@ -592,17 +603,17 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>60</v>
       </c>
@@ -644,15 +655,21 @@
         <v>5</v>
       </c>
       <c r="N3">
+        <v>0.8</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
         <v>19</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>25</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>61</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
put percentage and multiplier next to units,prices, and the other array stuff
</commit_message>
<xml_diff>
--- a/productImportExample.xlsx
+++ b/productImportExample.xlsx
@@ -491,14 +491,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="18.21875" customWidth="1"/>
-    <col min="13" max="15" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
     <col min="16" max="16" width="15.33203125" customWidth="1"/>
     <col min="17" max="17" width="20.77734375" customWidth="1"/>
     <col min="18" max="18" width="14.88671875" customWidth="1"/>
@@ -539,19 +542,19 @@
         <v>31</v>
       </c>
       <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
       </c>
       <c r="P1" t="s">
         <v>21</v>
@@ -597,10 +600,10 @@
       <c r="J2">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
@@ -645,20 +648,14 @@
       <c r="J3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>15</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>5</v>
-      </c>
-      <c r="N3">
-        <v>0.8</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
       </c>
       <c r="P3">
         <v>19</v>

</xml_diff>